<commit_message>
Corrected Net class SD_HST0, changed configuration for HW camera sync
</commit_message>
<xml_diff>
--- a/DM1097_DepthAI_Compute_Module_4/Docs/Assembly Outputs/BOM/BOM-DM1097_ACTIVE_BOM(Production).xlsx
+++ b/DM1097_DepthAI_Compute_Module_4/Docs/Assembly Outputs/BOM/BOM-DM1097_ACTIVE_BOM(Production).xlsx
@@ -1,43 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\02_Projects\DM1097_R0M0E0\KingTop_Output_Files\Assembly Outputs\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB6E5B3-7E2F-4E6E-86BD-A4E1C210B561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{68FD26FD-6D96-413A-9F12-C8F21D6EFB3E}"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="37395" windowHeight="19995"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-DM1097_ACTIVE_BOM(Productio" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'BOM-DM1097_ACTIVE_BOM(Productio'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="313">
   <si>
     <t>Name</t>
   </si>
@@ -706,7 +688,7 @@
     <t>0R 0603</t>
   </si>
   <si>
-    <t>R19, R20, R21, R29, R80, R85, R90</t>
+    <t>R19, R20, R21, R29, R81, R83, R90</t>
   </si>
   <si>
     <t>RES SMD 0 OHM JUMPER 1/10W 0603 0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
@@ -982,14 +964,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1034,18 +1016,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,9 +1034,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1074,44 +1050,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1139,31 +1115,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1191,23 +1150,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1219,2135 +1161,2181 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A775E9E-E013-4698-9DB4-639A9B41020B}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="7" width="31.77734375" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="1">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>9</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="1">
         <v>2</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="3" t="s">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="1">
         <v>3</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="1">
         <v>6</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="1">
         <v>4</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="1">
         <v>6</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="1">
         <v>4</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="1">
         <v>15</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I42" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I43" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H44" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="1">
         <v>2</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I46" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47" s="1">
         <v>7</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B48" s="4">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G48" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="I48" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="1">
         <v>4</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="I49" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="1">
         <v>4</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="H50" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="I50" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B51" s="4">
-        <v>1</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="H51" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I51" s="3" t="s">
+      <c r="I51" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="I52" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B53" s="4">
-        <v>1</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I53" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B54" s="4">
-        <v>1</v>
-      </c>
-      <c r="C54" s="3" t="s">
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="I54" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="1">
         <v>8</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="I55" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56" s="1">
         <v>2</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="I56" s="3" t="s">
+      <c r="I56" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57" s="1">
         <v>2</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H57" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="I57" s="3" t="s">
+      <c r="I57" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B58" s="4">
-        <v>1</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F58" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="H58" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="I58" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B59" s="4">
-        <v>1</v>
-      </c>
-      <c r="C59" s="3" t="s">
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G59" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="H59" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="I59" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B60" s="4">
-        <v>1</v>
-      </c>
-      <c r="C60" s="3" t="s">
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G60" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H60" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="I60" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B61" s="4">
-        <v>1</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H61" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="I61" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="H62" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="I62" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B63" s="4">
-        <v>1</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="H63" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I63" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B64" s="4">
-        <v>1</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="H64" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I64" s="3" t="s">
+      <c r="I64" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B65" s="4">
-        <v>1</v>
-      </c>
-      <c r="C65" s="3" t="s">
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F65" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="I65" s="3" t="s">
+      <c r="I65" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B66" s="4">
-        <v>1</v>
-      </c>
-      <c r="C66" s="3" t="s">
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="H66" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="I66" s="3" t="s">
+      <c r="I66" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B67" s="4">
-        <v>1</v>
-      </c>
-      <c r="C67" s="3" t="s">
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="H67" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="I67" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="3" t="s">
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I68" s="2" t="s">
         <v>312</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="22" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>